<commit_message>
change input data for 7 node
</commit_message>
<xml_diff>
--- a/input-fixed-nodes-temperatures.xlsx
+++ b/input-fixed-nodes-temperatures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xTEMP\PGU\payan-nameh-laptop\020-mc-dara-excel-to-matlab\excell-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xTEMP\PGU\payan-nameh-laptop\020-check-new-algorithm-for-7-nodes\excell-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79843C75-2F40-4944-8765-5CF990AE256E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41E95E7-AB82-4AD2-A013-A80BF9D2E332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -350,15 +350,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>132</v>
-      </c>
-      <c r="B2">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>